<commit_message>
Changed a wrong operation symbol (from '-' to '+')
</commit_message>
<xml_diff>
--- a/Module9.xlsx
+++ b/Module9.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nando\Documents\Kuliah\Semester 4\PSD\ProyekModul9\Implementasi-VHDL-1-100-Doors-\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{712BCC67-9148-45A1-B8D9-14F44EB745E6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{224E62F6-B38B-42F9-9510-0D312AFB2F87}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{029F5B94-1343-472B-8DF9-1892A7E04ED4}"/>
   </bookViews>
@@ -275,6 +275,9 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -284,7 +287,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
@@ -294,9 +297,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -615,8 +615,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A6F7A4B-4C50-48A0-B952-70304991B683}">
   <dimension ref="A1:J35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="80" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+    <sheetView tabSelected="1" zoomScale="80" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -629,18 +629,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A1" s="18" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18" t="s">
+      <c r="A1" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="18" t="s">
+      <c r="F1" s="15" t="s">
         <v>3</v>
       </c>
       <c r="I1" s="9" t="s">
@@ -649,7 +649,7 @@
       <c r="J1" s="9"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A2" s="18"/>
+      <c r="A2" s="15"/>
       <c r="B2" s="8" t="s">
         <v>5</v>
       </c>
@@ -659,8 +659,8 @@
       <c r="D2" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
       <c r="I2" s="2">
         <v>0</v>
       </c>
@@ -669,7 +669,7 @@
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="11" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="2">
@@ -678,13 +678,13 @@
       <c r="C3" s="2">
         <v>0</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="D3" s="12" t="s">
         <v>21</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="11">
+      <c r="F3" s="12">
         <v>1</v>
       </c>
       <c r="I3" s="2">
@@ -695,48 +695,48 @@
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A4" s="14"/>
+      <c r="A4" s="11"/>
       <c r="B4" s="2">
         <v>0</v>
       </c>
       <c r="C4" s="2">
         <v>1</v>
       </c>
-      <c r="D4" s="12"/>
-      <c r="E4" s="11" t="s">
+      <c r="D4" s="13"/>
+      <c r="E4" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="12"/>
+      <c r="F4" s="13"/>
       <c r="I4" s="4"/>
       <c r="J4" s="4"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A5" s="14"/>
+      <c r="A5" s="11"/>
       <c r="B5" s="2">
         <v>1</v>
       </c>
       <c r="C5" s="2">
         <v>0</v>
       </c>
-      <c r="D5" s="12"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13"/>
       <c r="I5" s="10" t="s">
         <v>13</v>
       </c>
       <c r="J5" s="10"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A6" s="14"/>
+      <c r="A6" s="11"/>
       <c r="B6" s="2">
         <v>1</v>
       </c>
       <c r="C6" s="2">
         <v>1</v>
       </c>
-      <c r="D6" s="13"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="13"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="14"/>
       <c r="I6" s="2">
         <v>0</v>
       </c>
@@ -745,7 +745,7 @@
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A7" s="14" t="s">
+      <c r="A7" s="11" t="s">
         <v>15</v>
       </c>
       <c r="B7" s="2">
@@ -754,7 +754,7 @@
       <c r="C7" s="2">
         <v>0</v>
       </c>
-      <c r="D7" s="11" t="s">
+      <c r="D7" s="12" t="s">
         <v>21</v>
       </c>
       <c r="E7" s="2" t="s">
@@ -771,49 +771,49 @@
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A8" s="14"/>
+      <c r="A8" s="11"/>
       <c r="B8" s="2">
         <v>0</v>
       </c>
       <c r="C8" s="2">
         <v>1</v>
       </c>
-      <c r="D8" s="12"/>
-      <c r="E8" s="11" t="s">
+      <c r="D8" s="13"/>
+      <c r="E8" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="F8" s="11">
+      <c r="F8" s="12">
         <v>1</v>
       </c>
       <c r="I8" s="5"/>
       <c r="J8" s="5"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A9" s="14"/>
+      <c r="A9" s="11"/>
       <c r="B9" s="2">
         <v>1</v>
       </c>
       <c r="C9" s="2">
         <v>0</v>
       </c>
-      <c r="D9" s="12"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="12"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A10" s="14"/>
+      <c r="A10" s="11"/>
       <c r="B10" s="2">
         <v>1</v>
       </c>
       <c r="C10" s="2">
         <v>1</v>
       </c>
-      <c r="D10" s="13"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="14"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A11" s="14" t="s">
+      <c r="A11" s="11" t="s">
         <v>11</v>
       </c>
       <c r="B11" s="2">
@@ -828,16 +828,16 @@
       <c r="E11" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F11" s="14">
+      <c r="F11" s="11">
         <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A12" s="14"/>
-      <c r="B12" s="11">
-        <v>0</v>
-      </c>
-      <c r="C12" s="11">
+      <c r="A12" s="11"/>
+      <c r="B12" s="12">
+        <v>0</v>
+      </c>
+      <c r="C12" s="12">
         <v>1</v>
       </c>
       <c r="D12" s="7">
@@ -846,58 +846,58 @@
       <c r="E12" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="F12" s="14"/>
+      <c r="F12" s="11"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A13" s="14"/>
-      <c r="B13" s="13"/>
-      <c r="C13" s="13"/>
+      <c r="A13" s="11"/>
+      <c r="B13" s="14"/>
+      <c r="C13" s="14"/>
       <c r="D13" s="7">
         <v>1</v>
       </c>
       <c r="E13" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="F13" s="14"/>
+      <c r="F13" s="11"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A14" s="14"/>
+      <c r="A14" s="11"/>
       <c r="B14" s="6">
         <v>1</v>
       </c>
       <c r="C14" s="6">
         <v>0</v>
       </c>
-      <c r="D14" s="11" t="s">
+      <c r="D14" s="12" t="s">
         <v>21</v>
       </c>
       <c r="E14" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="F14" s="14"/>
+      <c r="F14" s="11"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A15" s="14"/>
+      <c r="A15" s="11"/>
       <c r="B15" s="6">
         <v>1</v>
       </c>
       <c r="C15" s="6">
         <v>1</v>
       </c>
-      <c r="D15" s="13"/>
+      <c r="D15" s="14"/>
       <c r="E15" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="F15" s="14"/>
+      <c r="F15" s="11"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A16" s="15" t="s">
+      <c r="A16" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="B16" s="11">
-        <v>0</v>
-      </c>
-      <c r="C16" s="11">
+      <c r="B16" s="12">
+        <v>0</v>
+      </c>
+      <c r="C16" s="12">
         <v>0</v>
       </c>
       <c r="D16" s="6">
@@ -906,86 +906,86 @@
       <c r="E16" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="F16" s="11">
+      <c r="F16" s="12">
         <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A17" s="16"/>
-      <c r="B17" s="13"/>
-      <c r="C17" s="13"/>
+      <c r="A17" s="17"/>
+      <c r="B17" s="14"/>
+      <c r="C17" s="14"/>
       <c r="D17" s="6">
         <v>1</v>
       </c>
       <c r="E17" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="F17" s="12"/>
+      <c r="F17" s="13"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A18" s="16"/>
+      <c r="A18" s="17"/>
       <c r="B18" s="6">
         <v>0</v>
       </c>
       <c r="C18" s="6">
         <v>1</v>
       </c>
-      <c r="D18" s="11" t="s">
+      <c r="D18" s="12" t="s">
         <v>21</v>
       </c>
       <c r="E18" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="F18" s="12"/>
+      <c r="F18" s="13"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A19" s="16"/>
+      <c r="A19" s="17"/>
       <c r="B19" s="6">
         <v>1</v>
       </c>
       <c r="C19" s="6">
         <v>0</v>
       </c>
-      <c r="D19" s="13"/>
-      <c r="E19" s="11" t="s">
+      <c r="D19" s="14"/>
+      <c r="E19" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="F19" s="12"/>
+      <c r="F19" s="13"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A20" s="16"/>
-      <c r="B20" s="11">
-        <v>1</v>
-      </c>
-      <c r="C20" s="11">
+      <c r="A20" s="17"/>
+      <c r="B20" s="12">
+        <v>1</v>
+      </c>
+      <c r="C20" s="12">
         <v>1</v>
       </c>
       <c r="D20" s="6">
         <v>0</v>
       </c>
-      <c r="E20" s="13"/>
-      <c r="F20" s="12"/>
+      <c r="E20" s="14"/>
+      <c r="F20" s="13"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A21" s="17"/>
-      <c r="B21" s="13"/>
-      <c r="C21" s="13"/>
+      <c r="A21" s="18"/>
+      <c r="B21" s="14"/>
+      <c r="C21" s="14"/>
       <c r="D21" s="6">
         <v>1</v>
       </c>
       <c r="E21" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F21" s="13"/>
+      <c r="F21" s="14"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A22" s="11" t="s">
+      <c r="A22" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B22" s="11">
-        <v>0</v>
-      </c>
-      <c r="C22" s="11">
+      <c r="B22" s="12">
+        <v>0</v>
+      </c>
+      <c r="C22" s="12">
         <v>0</v>
       </c>
       <c r="D22" s="6">
@@ -994,58 +994,58 @@
       <c r="E22" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="F22" s="11">
+      <c r="F22" s="12">
         <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A23" s="12"/>
-      <c r="B23" s="13"/>
-      <c r="C23" s="13"/>
+      <c r="A23" s="13"/>
+      <c r="B23" s="14"/>
+      <c r="C23" s="14"/>
       <c r="D23" s="6">
         <v>1</v>
       </c>
       <c r="E23" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="F23" s="13"/>
+      <c r="F23" s="14"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A24" s="12"/>
+      <c r="A24" s="13"/>
       <c r="B24" s="6">
         <v>0</v>
       </c>
       <c r="C24" s="6">
         <v>1</v>
       </c>
-      <c r="D24" s="11" t="s">
+      <c r="D24" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="E24" s="11" t="s">
+      <c r="E24" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="F24" s="11">
+      <c r="F24" s="12">
         <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A25" s="12"/>
+      <c r="A25" s="13"/>
       <c r="B25" s="6">
         <v>1</v>
       </c>
       <c r="C25" s="6">
         <v>0</v>
       </c>
-      <c r="D25" s="13"/>
-      <c r="E25" s="13"/>
-      <c r="F25" s="13"/>
+      <c r="D25" s="14"/>
+      <c r="E25" s="14"/>
+      <c r="F25" s="14"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A26" s="12"/>
-      <c r="B26" s="11">
-        <v>1</v>
-      </c>
-      <c r="C26" s="11">
+      <c r="A26" s="13"/>
+      <c r="B26" s="12">
+        <v>1</v>
+      </c>
+      <c r="C26" s="12">
         <v>1</v>
       </c>
       <c r="D26" s="6">
@@ -1054,24 +1054,24 @@
       <c r="E26" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="F26" s="11">
+      <c r="F26" s="12">
         <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A27" s="13"/>
-      <c r="B27" s="13"/>
-      <c r="C27" s="13"/>
+      <c r="A27" s="14"/>
+      <c r="B27" s="14"/>
+      <c r="C27" s="14"/>
       <c r="D27" s="6">
         <v>1</v>
       </c>
       <c r="E27" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F27" s="13"/>
+      <c r="F27" s="14"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A28" s="14" t="s">
+      <c r="A28" s="11" t="s">
         <v>20</v>
       </c>
       <c r="B28" s="2">
@@ -1080,54 +1080,54 @@
       <c r="C28" s="2">
         <v>0</v>
       </c>
-      <c r="D28" s="11" t="s">
+      <c r="D28" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="E28" s="14" t="s">
+      <c r="E28" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="F28" s="14">
+      <c r="F28" s="11">
         <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A29" s="14"/>
+      <c r="A29" s="11"/>
       <c r="B29" s="2">
         <v>0</v>
       </c>
       <c r="C29" s="2">
         <v>1</v>
       </c>
-      <c r="D29" s="12"/>
-      <c r="E29" s="14"/>
-      <c r="F29" s="14"/>
+      <c r="D29" s="13"/>
+      <c r="E29" s="11"/>
+      <c r="F29" s="11"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A30" s="14"/>
+      <c r="A30" s="11"/>
       <c r="B30" s="2">
         <v>1</v>
       </c>
       <c r="C30" s="2">
         <v>0</v>
       </c>
-      <c r="D30" s="12"/>
-      <c r="E30" s="14"/>
-      <c r="F30" s="14"/>
+      <c r="D30" s="13"/>
+      <c r="E30" s="11"/>
+      <c r="F30" s="11"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A31" s="14"/>
+      <c r="A31" s="11"/>
       <c r="B31" s="2">
         <v>1</v>
       </c>
       <c r="C31" s="2">
         <v>1</v>
       </c>
-      <c r="D31" s="13"/>
-      <c r="E31" s="14"/>
-      <c r="F31" s="14"/>
+      <c r="D31" s="14"/>
+      <c r="E31" s="11"/>
+      <c r="F31" s="11"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A32" s="14" t="s">
+      <c r="A32" s="11" t="s">
         <v>17</v>
       </c>
       <c r="B32" s="2">
@@ -1136,74 +1136,64 @@
       <c r="C32" s="2">
         <v>0</v>
       </c>
-      <c r="D32" s="11" t="s">
+      <c r="D32" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="E32" s="14" t="s">
+      <c r="E32" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="F32" s="14" t="s">
+      <c r="F32" s="11" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A33" s="14"/>
+      <c r="A33" s="11"/>
       <c r="B33" s="2">
         <v>0</v>
       </c>
       <c r="C33" s="2">
         <v>1</v>
       </c>
-      <c r="D33" s="12"/>
-      <c r="E33" s="14"/>
-      <c r="F33" s="14"/>
+      <c r="D33" s="13"/>
+      <c r="E33" s="11"/>
+      <c r="F33" s="11"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A34" s="14"/>
+      <c r="A34" s="11"/>
       <c r="B34" s="2">
         <v>1</v>
       </c>
       <c r="C34" s="2">
         <v>0</v>
       </c>
-      <c r="D34" s="12"/>
-      <c r="E34" s="14"/>
-      <c r="F34" s="14"/>
+      <c r="D34" s="13"/>
+      <c r="E34" s="11"/>
+      <c r="F34" s="11"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A35" s="14"/>
+      <c r="A35" s="11"/>
       <c r="B35" s="2">
         <v>1</v>
       </c>
       <c r="C35" s="2">
         <v>1</v>
       </c>
-      <c r="D35" s="13"/>
-      <c r="E35" s="14"/>
-      <c r="F35" s="14"/>
+      <c r="D35" s="14"/>
+      <c r="E35" s="11"/>
+      <c r="F35" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="43">
-    <mergeCell ref="A32:A35"/>
-    <mergeCell ref="E32:E35"/>
-    <mergeCell ref="F32:F35"/>
-    <mergeCell ref="A28:A31"/>
-    <mergeCell ref="E28:E31"/>
-    <mergeCell ref="F28:F31"/>
-    <mergeCell ref="D28:D31"/>
-    <mergeCell ref="D32:D35"/>
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="F1:F2"/>
-    <mergeCell ref="A3:A6"/>
-    <mergeCell ref="A7:A10"/>
-    <mergeCell ref="F3:F6"/>
-    <mergeCell ref="D3:D6"/>
-    <mergeCell ref="D7:D10"/>
-    <mergeCell ref="F8:F10"/>
-    <mergeCell ref="E4:E6"/>
-    <mergeCell ref="E8:E10"/>
+    <mergeCell ref="A22:A27"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="C26:C27"/>
+    <mergeCell ref="F26:F27"/>
+    <mergeCell ref="F22:F23"/>
+    <mergeCell ref="F24:F25"/>
+    <mergeCell ref="E24:E25"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="C22:C23"/>
     <mergeCell ref="A11:A15"/>
     <mergeCell ref="A16:A21"/>
     <mergeCell ref="F16:F21"/>
@@ -1217,16 +1207,26 @@
     <mergeCell ref="B16:B17"/>
     <mergeCell ref="C16:C17"/>
     <mergeCell ref="F11:F15"/>
-    <mergeCell ref="A22:A27"/>
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="C26:C27"/>
-    <mergeCell ref="F26:F27"/>
-    <mergeCell ref="F22:F23"/>
-    <mergeCell ref="F24:F25"/>
-    <mergeCell ref="E24:E25"/>
-    <mergeCell ref="D24:D25"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="A7:A10"/>
+    <mergeCell ref="F3:F6"/>
+    <mergeCell ref="D3:D6"/>
+    <mergeCell ref="D7:D10"/>
+    <mergeCell ref="F8:F10"/>
+    <mergeCell ref="E4:E6"/>
+    <mergeCell ref="E8:E10"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="A3:A6"/>
+    <mergeCell ref="A32:A35"/>
+    <mergeCell ref="E32:E35"/>
+    <mergeCell ref="F32:F35"/>
+    <mergeCell ref="A28:A31"/>
+    <mergeCell ref="E28:E31"/>
+    <mergeCell ref="F28:F31"/>
+    <mergeCell ref="D28:D31"/>
+    <mergeCell ref="D32:D35"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Fixed border of table
</commit_message>
<xml_diff>
--- a/Module9.xlsx
+++ b/Module9.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nando\Documents\Kuliah\Semester 4\PSD\ProyekModul9\Implementasi-VHDL-1-100-Doors-\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{224E62F6-B38B-42F9-9510-0D312AFB2F87}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45CCD78E-5895-4050-B3AC-5F1C25E1FF10}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{029F5B94-1343-472B-8DF9-1892A7E04ED4}"/>
   </bookViews>
@@ -141,7 +141,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -178,19 +178,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -199,53 +186,11 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -259,16 +204,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -278,25 +214,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -616,7 +540,7 @@
   <dimension ref="A1:J35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -629,38 +553,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A1" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15" t="s">
+      <c r="A1" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="15" t="s">
+      <c r="F1" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="I1" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="J1" s="9"/>
+      <c r="J1" s="6"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A2" s="15"/>
-      <c r="B2" s="8" t="s">
+      <c r="A2" s="11"/>
+      <c r="B2" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
       <c r="I2" s="2">
         <v>0</v>
       </c>
@@ -669,22 +593,22 @@
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="2">
-        <v>0</v>
-      </c>
-      <c r="C3" s="2">
-        <v>0</v>
-      </c>
-      <c r="D3" s="12" t="s">
+      <c r="B3" s="8">
+        <v>0</v>
+      </c>
+      <c r="C3" s="8">
+        <v>0</v>
+      </c>
+      <c r="D3" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="12">
+      <c r="F3" s="10">
         <v>1</v>
       </c>
       <c r="I3" s="2">
@@ -695,48 +619,48 @@
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A4" s="11"/>
-      <c r="B4" s="2">
-        <v>0</v>
-      </c>
-      <c r="C4" s="2">
-        <v>1</v>
-      </c>
-      <c r="D4" s="13"/>
-      <c r="E4" s="12" t="s">
+      <c r="A4" s="10"/>
+      <c r="B4" s="8">
+        <v>0</v>
+      </c>
+      <c r="C4" s="8">
+        <v>1</v>
+      </c>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="13"/>
+      <c r="F4" s="10"/>
       <c r="I4" s="4"/>
       <c r="J4" s="4"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A5" s="11"/>
-      <c r="B5" s="2">
-        <v>1</v>
-      </c>
-      <c r="C5" s="2">
-        <v>0</v>
-      </c>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="13"/>
-      <c r="I5" s="10" t="s">
+      <c r="A5" s="10"/>
+      <c r="B5" s="8">
+        <v>1</v>
+      </c>
+      <c r="C5" s="8">
+        <v>0</v>
+      </c>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+      <c r="I5" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="J5" s="10"/>
+      <c r="J5" s="7"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A6" s="11"/>
-      <c r="B6" s="2">
-        <v>1</v>
-      </c>
-      <c r="C6" s="2">
-        <v>1</v>
-      </c>
-      <c r="D6" s="14"/>
-      <c r="E6" s="14"/>
-      <c r="F6" s="14"/>
+      <c r="A6" s="10"/>
+      <c r="B6" s="8">
+        <v>1</v>
+      </c>
+      <c r="C6" s="8">
+        <v>1</v>
+      </c>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="10"/>
       <c r="I6" s="2">
         <v>0</v>
       </c>
@@ -745,22 +669,22 @@
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A7" s="11" t="s">
+      <c r="A7" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="2">
-        <v>0</v>
-      </c>
-      <c r="C7" s="2">
-        <v>0</v>
-      </c>
-      <c r="D7" s="12" t="s">
+      <c r="B7" s="8">
+        <v>0</v>
+      </c>
+      <c r="C7" s="8">
+        <v>0</v>
+      </c>
+      <c r="D7" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="E7" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="F7" s="2">
+      <c r="F7" s="8">
         <v>0</v>
       </c>
       <c r="I7" s="3">
@@ -771,429 +695,439 @@
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A8" s="11"/>
-      <c r="B8" s="2">
-        <v>0</v>
-      </c>
-      <c r="C8" s="2">
-        <v>1</v>
-      </c>
-      <c r="D8" s="13"/>
-      <c r="E8" s="12" t="s">
+      <c r="A8" s="10"/>
+      <c r="B8" s="8">
+        <v>0</v>
+      </c>
+      <c r="C8" s="8">
+        <v>1</v>
+      </c>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="F8" s="12">
+      <c r="F8" s="10">
         <v>1</v>
       </c>
       <c r="I8" s="5"/>
       <c r="J8" s="5"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A9" s="11"/>
-      <c r="B9" s="2">
-        <v>1</v>
-      </c>
-      <c r="C9" s="2">
-        <v>0</v>
-      </c>
-      <c r="D9" s="13"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
+      <c r="A9" s="10"/>
+      <c r="B9" s="8">
+        <v>1</v>
+      </c>
+      <c r="C9" s="8">
+        <v>0</v>
+      </c>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A10" s="11"/>
-      <c r="B10" s="2">
-        <v>1</v>
-      </c>
-      <c r="C10" s="2">
-        <v>1</v>
-      </c>
-      <c r="D10" s="14"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="14"/>
+      <c r="A10" s="10"/>
+      <c r="B10" s="8">
+        <v>1</v>
+      </c>
+      <c r="C10" s="8">
+        <v>1</v>
+      </c>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A11" s="11" t="s">
+      <c r="A11" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="2">
-        <v>0</v>
-      </c>
-      <c r="C11" s="2">
-        <v>0</v>
-      </c>
-      <c r="D11" s="6" t="s">
+      <c r="B11" s="8">
+        <v>0</v>
+      </c>
+      <c r="C11" s="8">
+        <v>0</v>
+      </c>
+      <c r="D11" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="E11" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="F11" s="11">
+      <c r="F11" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A12" s="11"/>
-      <c r="B12" s="12">
-        <v>0</v>
-      </c>
-      <c r="C12" s="12">
-        <v>1</v>
-      </c>
-      <c r="D12" s="7">
-        <v>0</v>
-      </c>
-      <c r="E12" s="6" t="s">
+      <c r="A12" s="10"/>
+      <c r="B12" s="10">
+        <v>0</v>
+      </c>
+      <c r="C12" s="10">
+        <v>1</v>
+      </c>
+      <c r="D12" s="8">
+        <v>0</v>
+      </c>
+      <c r="E12" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="F12" s="11"/>
+      <c r="F12" s="10"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A13" s="11"/>
-      <c r="B13" s="14"/>
-      <c r="C13" s="14"/>
-      <c r="D13" s="7">
-        <v>1</v>
-      </c>
-      <c r="E13" s="6" t="s">
+      <c r="A13" s="10"/>
+      <c r="B13" s="10"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="8">
+        <v>1</v>
+      </c>
+      <c r="E13" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="F13" s="11"/>
+      <c r="F13" s="10"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A14" s="11"/>
-      <c r="B14" s="6">
-        <v>1</v>
-      </c>
-      <c r="C14" s="6">
-        <v>0</v>
-      </c>
-      <c r="D14" s="12" t="s">
+      <c r="A14" s="10"/>
+      <c r="B14" s="8">
+        <v>1</v>
+      </c>
+      <c r="C14" s="8">
+        <v>0</v>
+      </c>
+      <c r="D14" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="E14" s="6" t="s">
+      <c r="E14" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="F14" s="11"/>
+      <c r="F14" s="10"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A15" s="11"/>
-      <c r="B15" s="6">
-        <v>1</v>
-      </c>
-      <c r="C15" s="6">
-        <v>1</v>
-      </c>
-      <c r="D15" s="14"/>
-      <c r="E15" s="6" t="s">
+      <c r="A15" s="10"/>
+      <c r="B15" s="8">
+        <v>1</v>
+      </c>
+      <c r="C15" s="8">
+        <v>1</v>
+      </c>
+      <c r="D15" s="10"/>
+      <c r="E15" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="F15" s="11"/>
+      <c r="F15" s="10"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A16" s="16" t="s">
+      <c r="A16" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="B16" s="12">
-        <v>0</v>
-      </c>
-      <c r="C16" s="12">
-        <v>0</v>
-      </c>
-      <c r="D16" s="6">
-        <v>0</v>
-      </c>
-      <c r="E16" s="6" t="s">
+      <c r="B16" s="10">
+        <v>0</v>
+      </c>
+      <c r="C16" s="10">
+        <v>0</v>
+      </c>
+      <c r="D16" s="8">
+        <v>0</v>
+      </c>
+      <c r="E16" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="F16" s="12">
+      <c r="F16" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A17" s="17"/>
-      <c r="B17" s="14"/>
-      <c r="C17" s="14"/>
-      <c r="D17" s="6">
-        <v>1</v>
-      </c>
-      <c r="E17" s="6" t="s">
+      <c r="A17" s="10"/>
+      <c r="B17" s="10"/>
+      <c r="C17" s="10"/>
+      <c r="D17" s="8">
+        <v>1</v>
+      </c>
+      <c r="E17" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="F17" s="13"/>
+      <c r="F17" s="10"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A18" s="17"/>
-      <c r="B18" s="6">
-        <v>0</v>
-      </c>
-      <c r="C18" s="6">
-        <v>1</v>
-      </c>
-      <c r="D18" s="12" t="s">
+      <c r="A18" s="10"/>
+      <c r="B18" s="8">
+        <v>0</v>
+      </c>
+      <c r="C18" s="8">
+        <v>1</v>
+      </c>
+      <c r="D18" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="E18" s="6" t="s">
+      <c r="E18" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="F18" s="13"/>
+      <c r="F18" s="10"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A19" s="17"/>
-      <c r="B19" s="6">
-        <v>1</v>
-      </c>
-      <c r="C19" s="6">
-        <v>0</v>
-      </c>
-      <c r="D19" s="14"/>
-      <c r="E19" s="12" t="s">
+      <c r="A19" s="10"/>
+      <c r="B19" s="8">
+        <v>1</v>
+      </c>
+      <c r="C19" s="8">
+        <v>0</v>
+      </c>
+      <c r="D19" s="10"/>
+      <c r="E19" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="F19" s="13"/>
+      <c r="F19" s="10"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A20" s="17"/>
-      <c r="B20" s="12">
-        <v>1</v>
-      </c>
-      <c r="C20" s="12">
-        <v>1</v>
-      </c>
-      <c r="D20" s="6">
-        <v>0</v>
-      </c>
-      <c r="E20" s="14"/>
-      <c r="F20" s="13"/>
+      <c r="A20" s="10"/>
+      <c r="B20" s="10">
+        <v>1</v>
+      </c>
+      <c r="C20" s="10">
+        <v>1</v>
+      </c>
+      <c r="D20" s="8">
+        <v>0</v>
+      </c>
+      <c r="E20" s="10"/>
+      <c r="F20" s="10"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A21" s="18"/>
-      <c r="B21" s="14"/>
-      <c r="C21" s="14"/>
-      <c r="D21" s="6">
-        <v>1</v>
-      </c>
-      <c r="E21" s="2" t="s">
+      <c r="A21" s="10"/>
+      <c r="B21" s="10"/>
+      <c r="C21" s="10"/>
+      <c r="D21" s="8">
+        <v>1</v>
+      </c>
+      <c r="E21" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="F21" s="14"/>
+      <c r="F21" s="10"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A22" s="12" t="s">
+      <c r="A22" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="B22" s="12">
-        <v>0</v>
-      </c>
-      <c r="C22" s="12">
-        <v>0</v>
-      </c>
-      <c r="D22" s="6">
-        <v>0</v>
-      </c>
-      <c r="E22" s="2" t="s">
+      <c r="B22" s="10">
+        <v>0</v>
+      </c>
+      <c r="C22" s="10">
+        <v>0</v>
+      </c>
+      <c r="D22" s="8">
+        <v>0</v>
+      </c>
+      <c r="E22" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="F22" s="12">
+      <c r="F22" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A23" s="13"/>
-      <c r="B23" s="14"/>
-      <c r="C23" s="14"/>
-      <c r="D23" s="6">
-        <v>1</v>
-      </c>
-      <c r="E23" s="6" t="s">
+      <c r="A23" s="10"/>
+      <c r="B23" s="10"/>
+      <c r="C23" s="10"/>
+      <c r="D23" s="8">
+        <v>1</v>
+      </c>
+      <c r="E23" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="F23" s="14"/>
+      <c r="F23" s="10"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A24" s="13"/>
-      <c r="B24" s="6">
-        <v>0</v>
-      </c>
-      <c r="C24" s="6">
-        <v>1</v>
-      </c>
-      <c r="D24" s="12" t="s">
+      <c r="A24" s="10"/>
+      <c r="B24" s="8">
+        <v>0</v>
+      </c>
+      <c r="C24" s="8">
+        <v>1</v>
+      </c>
+      <c r="D24" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="E24" s="12" t="s">
+      <c r="E24" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="F24" s="12">
+      <c r="F24" s="10">
         <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A25" s="13"/>
-      <c r="B25" s="6">
-        <v>1</v>
-      </c>
-      <c r="C25" s="6">
-        <v>0</v>
-      </c>
-      <c r="D25" s="14"/>
-      <c r="E25" s="14"/>
-      <c r="F25" s="14"/>
+      <c r="A25" s="10"/>
+      <c r="B25" s="8">
+        <v>1</v>
+      </c>
+      <c r="C25" s="8">
+        <v>0</v>
+      </c>
+      <c r="D25" s="10"/>
+      <c r="E25" s="10"/>
+      <c r="F25" s="10"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A26" s="13"/>
-      <c r="B26" s="12">
-        <v>1</v>
-      </c>
-      <c r="C26" s="12">
-        <v>1</v>
-      </c>
-      <c r="D26" s="6">
-        <v>0</v>
-      </c>
-      <c r="E26" s="6" t="s">
+      <c r="A26" s="10"/>
+      <c r="B26" s="10">
+        <v>1</v>
+      </c>
+      <c r="C26" s="10">
+        <v>1</v>
+      </c>
+      <c r="D26" s="8">
+        <v>0</v>
+      </c>
+      <c r="E26" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="F26" s="12">
+      <c r="F26" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A27" s="14"/>
-      <c r="B27" s="14"/>
-      <c r="C27" s="14"/>
-      <c r="D27" s="6">
-        <v>1</v>
-      </c>
-      <c r="E27" s="2" t="s">
+      <c r="A27" s="10"/>
+      <c r="B27" s="10"/>
+      <c r="C27" s="10"/>
+      <c r="D27" s="8">
+        <v>1</v>
+      </c>
+      <c r="E27" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="F27" s="14"/>
+      <c r="F27" s="10"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A28" s="11" t="s">
+      <c r="A28" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="B28" s="2">
-        <v>0</v>
-      </c>
-      <c r="C28" s="2">
-        <v>0</v>
-      </c>
-      <c r="D28" s="12" t="s">
+      <c r="B28" s="8">
+        <v>0</v>
+      </c>
+      <c r="C28" s="8">
+        <v>0</v>
+      </c>
+      <c r="D28" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="E28" s="11" t="s">
+      <c r="E28" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="F28" s="11">
+      <c r="F28" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A29" s="11"/>
-      <c r="B29" s="2">
-        <v>0</v>
-      </c>
-      <c r="C29" s="2">
-        <v>1</v>
-      </c>
-      <c r="D29" s="13"/>
-      <c r="E29" s="11"/>
-      <c r="F29" s="11"/>
+      <c r="A29" s="10"/>
+      <c r="B29" s="8">
+        <v>0</v>
+      </c>
+      <c r="C29" s="8">
+        <v>1</v>
+      </c>
+      <c r="D29" s="10"/>
+      <c r="E29" s="10"/>
+      <c r="F29" s="10"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A30" s="11"/>
-      <c r="B30" s="2">
-        <v>1</v>
-      </c>
-      <c r="C30" s="2">
-        <v>0</v>
-      </c>
-      <c r="D30" s="13"/>
-      <c r="E30" s="11"/>
-      <c r="F30" s="11"/>
+      <c r="A30" s="10"/>
+      <c r="B30" s="8">
+        <v>1</v>
+      </c>
+      <c r="C30" s="8">
+        <v>0</v>
+      </c>
+      <c r="D30" s="10"/>
+      <c r="E30" s="10"/>
+      <c r="F30" s="10"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A31" s="11"/>
-      <c r="B31" s="2">
-        <v>1</v>
-      </c>
-      <c r="C31" s="2">
-        <v>1</v>
-      </c>
-      <c r="D31" s="14"/>
-      <c r="E31" s="11"/>
-      <c r="F31" s="11"/>
+      <c r="A31" s="10"/>
+      <c r="B31" s="8">
+        <v>1</v>
+      </c>
+      <c r="C31" s="8">
+        <v>1</v>
+      </c>
+      <c r="D31" s="10"/>
+      <c r="E31" s="10"/>
+      <c r="F31" s="10"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A32" s="11" t="s">
+      <c r="A32" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="B32" s="2">
-        <v>0</v>
-      </c>
-      <c r="C32" s="2">
-        <v>0</v>
-      </c>
-      <c r="D32" s="12" t="s">
+      <c r="B32" s="8">
+        <v>0</v>
+      </c>
+      <c r="C32" s="8">
+        <v>0</v>
+      </c>
+      <c r="D32" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="E32" s="11" t="s">
+      <c r="E32" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="F32" s="11" t="s">
+      <c r="F32" s="10" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A33" s="11"/>
-      <c r="B33" s="2">
-        <v>0</v>
-      </c>
-      <c r="C33" s="2">
-        <v>1</v>
-      </c>
-      <c r="D33" s="13"/>
-      <c r="E33" s="11"/>
-      <c r="F33" s="11"/>
+      <c r="A33" s="10"/>
+      <c r="B33" s="8">
+        <v>0</v>
+      </c>
+      <c r="C33" s="8">
+        <v>1</v>
+      </c>
+      <c r="D33" s="10"/>
+      <c r="E33" s="10"/>
+      <c r="F33" s="10"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A34" s="11"/>
-      <c r="B34" s="2">
-        <v>1</v>
-      </c>
-      <c r="C34" s="2">
-        <v>0</v>
-      </c>
-      <c r="D34" s="13"/>
-      <c r="E34" s="11"/>
-      <c r="F34" s="11"/>
+      <c r="A34" s="10"/>
+      <c r="B34" s="8">
+        <v>1</v>
+      </c>
+      <c r="C34" s="8">
+        <v>0</v>
+      </c>
+      <c r="D34" s="10"/>
+      <c r="E34" s="10"/>
+      <c r="F34" s="10"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A35" s="11"/>
-      <c r="B35" s="2">
-        <v>1</v>
-      </c>
-      <c r="C35" s="2">
-        <v>1</v>
-      </c>
-      <c r="D35" s="14"/>
-      <c r="E35" s="11"/>
-      <c r="F35" s="11"/>
+      <c r="A35" s="10"/>
+      <c r="B35" s="8">
+        <v>1</v>
+      </c>
+      <c r="C35" s="8">
+        <v>1</v>
+      </c>
+      <c r="D35" s="10"/>
+      <c r="E35" s="10"/>
+      <c r="F35" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="43">
-    <mergeCell ref="A22:A27"/>
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="C26:C27"/>
-    <mergeCell ref="F26:F27"/>
-    <mergeCell ref="F22:F23"/>
-    <mergeCell ref="F24:F25"/>
-    <mergeCell ref="E24:E25"/>
-    <mergeCell ref="D24:D25"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="A32:A35"/>
+    <mergeCell ref="E32:E35"/>
+    <mergeCell ref="F32:F35"/>
+    <mergeCell ref="A28:A31"/>
+    <mergeCell ref="E28:E31"/>
+    <mergeCell ref="F28:F31"/>
+    <mergeCell ref="D28:D31"/>
+    <mergeCell ref="D32:D35"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="A3:A6"/>
+    <mergeCell ref="A7:A10"/>
+    <mergeCell ref="F3:F6"/>
+    <mergeCell ref="D3:D6"/>
+    <mergeCell ref="D7:D10"/>
+    <mergeCell ref="F8:F10"/>
+    <mergeCell ref="E4:E6"/>
+    <mergeCell ref="E8:E10"/>
     <mergeCell ref="A11:A15"/>
     <mergeCell ref="A16:A21"/>
     <mergeCell ref="F16:F21"/>
@@ -1207,26 +1141,16 @@
     <mergeCell ref="B16:B17"/>
     <mergeCell ref="C16:C17"/>
     <mergeCell ref="F11:F15"/>
-    <mergeCell ref="A7:A10"/>
-    <mergeCell ref="F3:F6"/>
-    <mergeCell ref="D3:D6"/>
-    <mergeCell ref="D7:D10"/>
-    <mergeCell ref="F8:F10"/>
-    <mergeCell ref="E4:E6"/>
-    <mergeCell ref="E8:E10"/>
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="F1:F2"/>
-    <mergeCell ref="A3:A6"/>
-    <mergeCell ref="A32:A35"/>
-    <mergeCell ref="E32:E35"/>
-    <mergeCell ref="F32:F35"/>
-    <mergeCell ref="A28:A31"/>
-    <mergeCell ref="E28:E31"/>
-    <mergeCell ref="F28:F31"/>
-    <mergeCell ref="D28:D31"/>
-    <mergeCell ref="D32:D35"/>
+    <mergeCell ref="A22:A27"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="C26:C27"/>
+    <mergeCell ref="F26:F27"/>
+    <mergeCell ref="F22:F23"/>
+    <mergeCell ref="F24:F25"/>
+    <mergeCell ref="E24:E25"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="C22:C23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>